<commit_message>
updateProfile and add MNT
</commit_message>
<xml_diff>
--- a/Document/WebTours_Профиль_нагрузки.xlsx
+++ b/Document/WebTours_Профиль_нагрузки.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Автоматизированный расчет" sheetId="3" r:id="rId1"/>
@@ -970,7 +970,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -1492,6 +1492,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1643,7 +1667,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -1784,6 +1808,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="134"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="134"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1793,8 +1819,33 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="134"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="134"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="148">
     <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2742,10 +2793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X75"/>
+  <dimension ref="A1:X76"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2769,6 +2820,7 @@
     <col min="17" max="17" width="26" customWidth="1"/>
     <col min="18" max="18" width="10.42578125" customWidth="1"/>
     <col min="19" max="19" width="12.28515625" customWidth="1"/>
+    <col min="21" max="21" width="23.42578125" customWidth="1"/>
     <col min="22" max="22" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3259,8 +3311,8 @@
         <v>20</v>
       </c>
       <c r="U7" s="9">
-        <f>SUM(U2:U6)</f>
-        <v>160</v>
+        <f>ROUND(R7*S7*T7,0)</f>
+        <v>12</v>
       </c>
       <c r="V7" s="18">
         <f t="shared" si="5"/>
@@ -3728,8 +3780,8 @@
       <c r="A21" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>3</v>
+      <c r="B21" s="68" t="s">
+        <v>46</v>
       </c>
       <c r="C21" s="52">
         <v>1</v>
@@ -3759,8 +3811,8 @@
       <c r="A22" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="68" t="s">
-        <v>46</v>
+      <c r="B22" s="51" t="s">
+        <v>3</v>
       </c>
       <c r="C22" s="58">
         <v>1</v>
@@ -4097,10 +4149,10 @@
     </row>
     <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="94" t="s">
+      <c r="A36" s="96" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="95"/>
+      <c r="B36" s="97"/>
     </row>
     <row r="37" spans="1:9" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
@@ -4566,107 +4618,169 @@
       <c r="G52" s="17"/>
       <c r="H52" s="17"/>
     </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="91"/>
+      <c r="B58" s="91"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="91"/>
+      <c r="B59" s="91"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="80"/>
+      <c r="B60" s="80"/>
+      <c r="C60" s="80"/>
+    </row>
     <row r="61" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A61" s="74"/>
+      <c r="B61" s="74"/>
+      <c r="C61" s="80"/>
       <c r="K61" s="85"/>
       <c r="L61" s="74"/>
       <c r="M61" s="81"/>
       <c r="N61" s="74"/>
       <c r="O61" s="73"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="74"/>
+      <c r="B62" s="103"/>
+      <c r="C62" s="80"/>
       <c r="K62" s="79"/>
       <c r="L62" s="77"/>
       <c r="M62" s="82"/>
       <c r="N62" s="75"/>
       <c r="O62" s="73"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="106"/>
+      <c r="B63" s="103"/>
+      <c r="C63" s="80"/>
       <c r="K63" s="79"/>
       <c r="L63" s="77"/>
       <c r="M63" s="83"/>
       <c r="N63" s="76"/>
       <c r="O63" s="78"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="106"/>
+      <c r="B64" s="103"/>
+      <c r="C64" s="80"/>
       <c r="K64" s="79"/>
       <c r="L64" s="77"/>
       <c r="M64" s="82"/>
       <c r="N64" s="75"/>
       <c r="O64" s="79"/>
     </row>
-    <row r="65" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="107"/>
+      <c r="B65" s="108"/>
+      <c r="C65" s="80"/>
       <c r="K65" s="79"/>
       <c r="L65" s="77"/>
       <c r="M65" s="82"/>
       <c r="N65" s="75"/>
       <c r="O65" s="79"/>
     </row>
-    <row r="66" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="107"/>
+      <c r="B66" s="108"/>
+      <c r="C66" s="80"/>
       <c r="K66" s="79"/>
       <c r="L66" s="77"/>
       <c r="M66" s="82"/>
       <c r="N66" s="75"/>
       <c r="O66" s="79"/>
     </row>
-    <row r="67" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="107"/>
+      <c r="B67" s="108"/>
+      <c r="C67" s="80"/>
       <c r="K67" s="79"/>
       <c r="L67" s="77"/>
       <c r="M67" s="82"/>
       <c r="N67" s="75"/>
       <c r="O67" s="79"/>
     </row>
-    <row r="68" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="107"/>
+      <c r="B68" s="108"/>
+      <c r="C68" s="80"/>
       <c r="K68" s="79"/>
       <c r="L68" s="77"/>
       <c r="M68" s="82"/>
       <c r="N68" s="75"/>
       <c r="O68" s="79"/>
     </row>
-    <row r="69" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="107"/>
+      <c r="B69" s="108"/>
+      <c r="C69" s="80"/>
       <c r="K69" s="79"/>
       <c r="L69" s="77"/>
       <c r="M69" s="82"/>
       <c r="N69" s="75"/>
       <c r="O69" s="79"/>
     </row>
-    <row r="70" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="106"/>
+      <c r="B70" s="103"/>
+      <c r="C70" s="80"/>
       <c r="K70" s="79"/>
       <c r="L70" s="77"/>
       <c r="M70" s="82"/>
       <c r="N70" s="75"/>
       <c r="O70" s="79"/>
     </row>
-    <row r="71" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="109"/>
+      <c r="B71" s="102"/>
+      <c r="C71" s="80"/>
       <c r="K71" s="79"/>
       <c r="L71" s="77"/>
       <c r="M71" s="82"/>
       <c r="N71" s="75"/>
       <c r="O71" s="79"/>
     </row>
-    <row r="72" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="109"/>
+      <c r="B72" s="102"/>
+      <c r="C72" s="80"/>
       <c r="K72" s="79"/>
       <c r="L72" s="77"/>
       <c r="M72" s="82"/>
       <c r="N72" s="75"/>
       <c r="O72" s="79"/>
     </row>
-    <row r="73" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="109"/>
+      <c r="B73" s="102"/>
+      <c r="C73" s="80"/>
       <c r="K73" s="79"/>
       <c r="L73" s="77"/>
       <c r="M73" s="82"/>
       <c r="N73" s="75"/>
       <c r="O73" s="79"/>
     </row>
-    <row r="74" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="104"/>
+      <c r="B74" s="105"/>
+      <c r="C74" s="99"/>
       <c r="K74" s="80"/>
       <c r="L74" s="80"/>
       <c r="M74" s="84"/>
       <c r="N74" s="80"/>
       <c r="O74" s="80"/>
     </row>
-    <row r="75" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" s="100"/>
+      <c r="B75" s="79"/>
+      <c r="C75" s="101"/>
       <c r="K75" s="80"/>
       <c r="L75" s="80"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" s="72"/>
+      <c r="B76" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4866,578 +4980,578 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="97">
+      <c r="C2" s="94">
         <v>0.124</v>
       </c>
-      <c r="D2" s="97">
+      <c r="D2" s="94">
         <v>0.153</v>
       </c>
-      <c r="E2" s="97">
+      <c r="E2" s="94">
         <v>0.20300000000000001</v>
       </c>
-      <c r="F2" s="97">
+      <c r="F2" s="94">
         <v>2.3E-2</v>
       </c>
-      <c r="G2" s="97">
+      <c r="G2" s="94">
         <v>0.17599999999999999</v>
       </c>
-      <c r="H2" s="97">
+      <c r="H2" s="94">
         <v>93</v>
       </c>
-      <c r="I2" s="97">
-        <v>0</v>
-      </c>
-      <c r="J2" s="97">
+      <c r="I2" s="94">
+        <v>0</v>
+      </c>
+      <c r="J2" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="97">
+      <c r="C3" s="94">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="D3" s="97">
+      <c r="D3" s="94">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="E3" s="97">
+      <c r="E3" s="94">
         <v>0.121</v>
       </c>
-      <c r="F3" s="97">
+      <c r="F3" s="94">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="G3" s="97">
+      <c r="G3" s="94">
         <v>0.1</v>
       </c>
-      <c r="H3" s="97">
+      <c r="H3" s="94">
         <v>25</v>
       </c>
-      <c r="I3" s="97">
-        <v>0</v>
-      </c>
-      <c r="J3" s="97">
+      <c r="I3" s="94">
+        <v>0</v>
+      </c>
+      <c r="J3" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="97" t="s">
+      <c r="A4" s="94" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="97">
+      <c r="C4" s="94">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D4" s="97">
+      <c r="D4" s="94">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="E4" s="97">
+      <c r="E4" s="94">
         <v>0.11700000000000001</v>
       </c>
-      <c r="F4" s="97">
+      <c r="F4" s="94">
         <v>2.3E-2</v>
       </c>
-      <c r="G4" s="97">
+      <c r="G4" s="94">
         <v>0.10199999999999999</v>
       </c>
-      <c r="H4" s="97">
+      <c r="H4" s="94">
         <v>94</v>
       </c>
-      <c r="I4" s="97">
-        <v>0</v>
-      </c>
-      <c r="J4" s="97">
+      <c r="I4" s="94">
+        <v>0</v>
+      </c>
+      <c r="J4" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="97" t="s">
+      <c r="A5" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="97">
+      <c r="C5" s="94">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="D5" s="97">
+      <c r="D5" s="94">
         <v>0.122</v>
       </c>
-      <c r="E5" s="97">
+      <c r="E5" s="94">
         <v>0.19</v>
       </c>
-      <c r="F5" s="97">
+      <c r="F5" s="94">
         <v>2.3E-2</v>
       </c>
-      <c r="G5" s="97">
+      <c r="G5" s="94">
         <v>0.14399999999999999</v>
       </c>
-      <c r="H5" s="97">
+      <c r="H5" s="94">
         <v>140</v>
       </c>
-      <c r="I5" s="97">
-        <v>0</v>
-      </c>
-      <c r="J5" s="97">
+      <c r="I5" s="94">
+        <v>0</v>
+      </c>
+      <c r="J5" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="97">
+      <c r="C6" s="94">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="D6" s="97">
+      <c r="D6" s="94">
         <v>0.10299999999999999</v>
       </c>
-      <c r="E6" s="97">
+      <c r="E6" s="94">
         <v>0.13900000000000001</v>
       </c>
-      <c r="F6" s="97">
+      <c r="F6" s="94">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="G6" s="97">
+      <c r="G6" s="94">
         <v>0.129</v>
       </c>
-      <c r="H6" s="97">
+      <c r="H6" s="94">
         <v>117</v>
       </c>
-      <c r="I6" s="97">
-        <v>0</v>
-      </c>
-      <c r="J6" s="97">
+      <c r="I6" s="94">
+        <v>0</v>
+      </c>
+      <c r="J6" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="97" t="s">
+      <c r="A7" s="94" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="97">
+      <c r="C7" s="94">
         <v>4.7E-2</v>
       </c>
-      <c r="D7" s="97">
+      <c r="D7" s="94">
         <v>7.8E-2</v>
       </c>
-      <c r="E7" s="97">
+      <c r="E7" s="94">
         <v>0.13</v>
       </c>
-      <c r="F7" s="97">
+      <c r="F7" s="94">
         <v>2.4E-2</v>
       </c>
-      <c r="G7" s="97">
+      <c r="G7" s="94">
         <v>0.10299999999999999</v>
       </c>
-      <c r="H7" s="97">
+      <c r="H7" s="94">
         <v>58</v>
       </c>
-      <c r="I7" s="97">
-        <v>0</v>
-      </c>
-      <c r="J7" s="97">
+      <c r="I7" s="94">
+        <v>0</v>
+      </c>
+      <c r="J7" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="97" t="s">
+      <c r="A8" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="97" t="s">
+      <c r="B8" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="97">
+      <c r="C8" s="94">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="D8" s="97">
+      <c r="D8" s="94">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="E8" s="97">
+      <c r="E8" s="94">
         <v>0.106</v>
       </c>
-      <c r="F8" s="97">
+      <c r="F8" s="94">
         <v>2.4E-2</v>
       </c>
-      <c r="G8" s="97">
+      <c r="G8" s="94">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="H8" s="97">
+      <c r="H8" s="94">
         <v>34</v>
       </c>
-      <c r="I8" s="97">
-        <v>0</v>
-      </c>
-      <c r="J8" s="97">
+      <c r="I8" s="94">
+        <v>0</v>
+      </c>
+      <c r="J8" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="97" t="s">
+      <c r="A9" s="94" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="97">
+      <c r="C9" s="94">
         <v>4.7E-2</v>
       </c>
-      <c r="D9" s="97">
+      <c r="D9" s="94">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="E9" s="97">
+      <c r="E9" s="94">
         <v>0.113</v>
       </c>
-      <c r="F9" s="97">
+      <c r="F9" s="94">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="G9" s="97">
+      <c r="G9" s="94">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="H9" s="97">
+      <c r="H9" s="94">
         <v>94</v>
       </c>
-      <c r="I9" s="97">
-        <v>0</v>
-      </c>
-      <c r="J9" s="97">
+      <c r="I9" s="94">
+        <v>0</v>
+      </c>
+      <c r="J9" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="97" t="s">
+      <c r="A10" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="97" t="s">
+      <c r="B10" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="97">
+      <c r="C10" s="94">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="D10" s="97">
+      <c r="D10" s="94">
         <v>0.107</v>
       </c>
-      <c r="E10" s="97">
+      <c r="E10" s="94">
         <v>0.17899999999999999</v>
       </c>
-      <c r="F10" s="97">
+      <c r="F10" s="94">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="G10" s="97">
+      <c r="G10" s="94">
         <v>0.13300000000000001</v>
       </c>
-      <c r="H10" s="97">
+      <c r="H10" s="94">
         <v>170</v>
       </c>
-      <c r="I10" s="97">
-        <v>0</v>
-      </c>
-      <c r="J10" s="97">
+      <c r="I10" s="94">
+        <v>0</v>
+      </c>
+      <c r="J10" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="97" t="s">
+      <c r="A11" s="94" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="97" t="s">
+      <c r="B11" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="97">
+      <c r="C11" s="94">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="D11" s="97">
+      <c r="D11" s="94">
         <v>0.122</v>
       </c>
-      <c r="E11" s="97">
+      <c r="E11" s="94">
         <v>0.159</v>
       </c>
-      <c r="F11" s="97">
+      <c r="F11" s="94">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="G11" s="97">
+      <c r="G11" s="94">
         <v>0.14299999999999999</v>
       </c>
-      <c r="H11" s="97">
+      <c r="H11" s="94">
         <v>34</v>
       </c>
-      <c r="I11" s="97">
-        <v>0</v>
-      </c>
-      <c r="J11" s="97">
+      <c r="I11" s="94">
+        <v>0</v>
+      </c>
+      <c r="J11" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="97" t="s">
+      <c r="A12" s="94" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="97" t="s">
+      <c r="B12" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="97">
+      <c r="C12" s="94">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="D12" s="97">
+      <c r="D12" s="94">
         <v>0.151</v>
       </c>
-      <c r="E12" s="97">
+      <c r="E12" s="94">
         <v>0.20100000000000001</v>
       </c>
-      <c r="F12" s="97">
+      <c r="F12" s="94">
         <v>2.4E-2</v>
       </c>
-      <c r="G12" s="97">
+      <c r="G12" s="94">
         <v>0.17599999999999999</v>
       </c>
-      <c r="H12" s="97">
+      <c r="H12" s="94">
         <v>106</v>
       </c>
-      <c r="I12" s="97">
-        <v>0</v>
-      </c>
-      <c r="J12" s="97">
+      <c r="I12" s="94">
+        <v>0</v>
+      </c>
+      <c r="J12" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="97" t="s">
+      <c r="A13" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="97" t="s">
+      <c r="B13" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="97">
+      <c r="C13" s="94">
         <v>7.8E-2</v>
       </c>
-      <c r="D13" s="97">
+      <c r="D13" s="94">
         <v>0.107</v>
       </c>
-      <c r="E13" s="97">
+      <c r="E13" s="94">
         <v>0.13500000000000001</v>
       </c>
-      <c r="F13" s="97">
+      <c r="F13" s="94">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="G13" s="97">
+      <c r="G13" s="94">
         <v>0.13100000000000001</v>
       </c>
-      <c r="H13" s="97">
+      <c r="H13" s="94">
         <v>33</v>
       </c>
-      <c r="I13" s="97">
-        <v>0</v>
-      </c>
-      <c r="J13" s="97">
+      <c r="I13" s="94">
+        <v>0</v>
+      </c>
+      <c r="J13" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="97" t="s">
+      <c r="A14" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="97" t="s">
+      <c r="B14" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="97">
+      <c r="C14" s="94">
         <v>0.57099999999999995</v>
       </c>
-      <c r="D14" s="97">
+      <c r="D14" s="94">
         <v>0.754</v>
       </c>
-      <c r="E14" s="97">
+      <c r="E14" s="94">
         <v>0.91500000000000004</v>
       </c>
-      <c r="F14" s="97">
+      <c r="F14" s="94">
         <v>0.11799999999999999</v>
       </c>
-      <c r="G14" s="97">
+      <c r="G14" s="94">
         <v>0.88900000000000001</v>
       </c>
-      <c r="H14" s="97">
+      <c r="H14" s="94">
         <v>57</v>
       </c>
-      <c r="I14" s="97">
-        <v>0</v>
-      </c>
-      <c r="J14" s="97">
+      <c r="I14" s="94">
+        <v>0</v>
+      </c>
+      <c r="J14" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="94" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="97" t="s">
+      <c r="B15" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="97">
+      <c r="C15" s="94">
         <v>0.374</v>
       </c>
-      <c r="D15" s="97">
+      <c r="D15" s="94">
         <v>0.503</v>
       </c>
-      <c r="E15" s="97">
+      <c r="E15" s="94">
         <v>0.64200000000000002</v>
       </c>
-      <c r="F15" s="97">
+      <c r="F15" s="94">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="G15" s="97">
+      <c r="G15" s="94">
         <v>0.60899999999999999</v>
       </c>
-      <c r="H15" s="97">
+      <c r="H15" s="94">
         <v>33</v>
       </c>
-      <c r="I15" s="97">
-        <v>0</v>
-      </c>
-      <c r="J15" s="97">
+      <c r="I15" s="94">
+        <v>0</v>
+      </c>
+      <c r="J15" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="97" t="s">
+      <c r="A16" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="B16" s="97" t="s">
+      <c r="B16" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="97">
+      <c r="C16" s="94">
         <v>0.47399999999999998</v>
       </c>
-      <c r="D16" s="97">
+      <c r="D16" s="94">
         <v>0.63500000000000001</v>
       </c>
-      <c r="E16" s="97">
+      <c r="E16" s="94">
         <v>0.81</v>
       </c>
-      <c r="F16" s="97">
+      <c r="F16" s="94">
         <v>0.10100000000000001</v>
       </c>
-      <c r="G16" s="97">
+      <c r="G16" s="94">
         <v>0.751</v>
       </c>
-      <c r="H16" s="97">
+      <c r="H16" s="94">
         <v>36</v>
       </c>
-      <c r="I16" s="97">
-        <v>0</v>
-      </c>
-      <c r="J16" s="97">
+      <c r="I16" s="94">
+        <v>0</v>
+      </c>
+      <c r="J16" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="97" t="s">
+      <c r="A17" s="94" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="97" t="s">
+      <c r="B17" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="97">
+      <c r="C17" s="94">
         <v>0.435</v>
       </c>
-      <c r="D17" s="97">
+      <c r="D17" s="94">
         <v>0.54500000000000004</v>
       </c>
-      <c r="E17" s="97">
+      <c r="E17" s="94">
         <v>0.65600000000000003</v>
       </c>
-      <c r="F17" s="97">
+      <c r="F17" s="94">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="G17" s="97">
+      <c r="G17" s="94">
         <v>0.65400000000000003</v>
       </c>
-      <c r="H17" s="97">
+      <c r="H17" s="94">
         <v>25</v>
       </c>
-      <c r="I17" s="97">
-        <v>0</v>
-      </c>
-      <c r="J17" s="97">
+      <c r="I17" s="94">
+        <v>0</v>
+      </c>
+      <c r="J17" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="97" t="s">
+      <c r="A18" s="94" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="97" t="s">
+      <c r="B18" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="97">
+      <c r="C18" s="94">
         <v>0.38400000000000001</v>
       </c>
-      <c r="D18" s="97">
+      <c r="D18" s="94">
         <v>0.49399999999999999</v>
       </c>
-      <c r="E18" s="97">
+      <c r="E18" s="94">
         <v>0.63100000000000001</v>
       </c>
-      <c r="F18" s="97">
+      <c r="F18" s="94">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="G18" s="97">
+      <c r="G18" s="94">
         <v>0.58199999999999996</v>
       </c>
-      <c r="H18" s="97">
+      <c r="H18" s="94">
         <v>11</v>
       </c>
-      <c r="I18" s="97">
-        <v>0</v>
-      </c>
-      <c r="J18" s="97">
+      <c r="I18" s="94">
+        <v>0</v>
+      </c>
+      <c r="J18" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="97" t="s">
+      <c r="A19" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="97" t="s">
+      <c r="B19" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="97">
+      <c r="C19" s="94">
         <v>0.378</v>
       </c>
-      <c r="D19" s="97">
+      <c r="D19" s="94">
         <v>0.52400000000000002</v>
       </c>
-      <c r="E19" s="97">
+      <c r="E19" s="94">
         <v>0.58899999999999997</v>
       </c>
-      <c r="F19" s="97">
+      <c r="F19" s="94">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="G19" s="97">
+      <c r="G19" s="94">
         <v>0.58799999999999997</v>
       </c>
-      <c r="H19" s="97">
+      <c r="H19" s="94">
         <v>12</v>
       </c>
-      <c r="I19" s="97">
-        <v>0</v>
-      </c>
-      <c r="J19" s="97">
+      <c r="I19" s="94">
+        <v>0</v>
+      </c>
+      <c r="J19" s="94">
         <v>0</v>
       </c>
     </row>
@@ -5504,578 +5618,578 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="98">
+      <c r="C2" s="95">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="D2" s="98">
+      <c r="D2" s="95">
         <v>0.19</v>
       </c>
-      <c r="E2" s="98">
+      <c r="E2" s="95">
         <v>2.1469999999999998</v>
       </c>
-      <c r="F2" s="98">
+      <c r="F2" s="95">
         <v>0.182</v>
       </c>
-      <c r="G2" s="98">
+      <c r="G2" s="95">
         <v>0.191</v>
       </c>
-      <c r="H2" s="98">
+      <c r="H2" s="95">
         <v>281</v>
       </c>
-      <c r="I2" s="98">
-        <v>0</v>
-      </c>
-      <c r="J2" s="98">
+      <c r="I2" s="95">
+        <v>0</v>
+      </c>
+      <c r="J2" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="98">
+      <c r="C3" s="95">
         <v>4.7E-2</v>
       </c>
-      <c r="D3" s="98">
+      <c r="D3" s="95">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="E3" s="98">
+      <c r="E3" s="95">
         <v>0.20799999999999999</v>
       </c>
-      <c r="F3" s="98">
+      <c r="F3" s="95">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="G3" s="98">
+      <c r="G3" s="95">
         <v>0.107</v>
       </c>
-      <c r="H3" s="98">
+      <c r="H3" s="95">
         <v>75</v>
       </c>
-      <c r="I3" s="98">
-        <v>0</v>
-      </c>
-      <c r="J3" s="98">
+      <c r="I3" s="95">
+        <v>0</v>
+      </c>
+      <c r="J3" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="98" t="s">
+      <c r="A4" s="95" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="98">
+      <c r="C4" s="95">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D4" s="98">
+      <c r="D4" s="95">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="E4" s="98">
+      <c r="E4" s="95">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F4" s="98">
+      <c r="F4" s="95">
         <v>0.104</v>
       </c>
-      <c r="G4" s="98">
+      <c r="G4" s="95">
         <v>0.106</v>
       </c>
-      <c r="H4" s="98">
+      <c r="H4" s="95">
         <v>278</v>
       </c>
-      <c r="I4" s="98">
-        <v>0</v>
-      </c>
-      <c r="J4" s="98">
+      <c r="I4" s="95">
+        <v>0</v>
+      </c>
+      <c r="J4" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="98" t="s">
+      <c r="A5" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="98">
+      <c r="C5" s="95">
         <v>0.09</v>
       </c>
-      <c r="D5" s="98">
+      <c r="D5" s="95">
         <v>0.185</v>
       </c>
-      <c r="E5" s="98">
+      <c r="E5" s="95">
         <v>2.1629999999999998</v>
       </c>
-      <c r="F5" s="98">
+      <c r="F5" s="95">
         <v>0.25900000000000001</v>
       </c>
-      <c r="G5" s="98">
+      <c r="G5" s="95">
         <v>0.16700000000000001</v>
       </c>
-      <c r="H5" s="98">
+      <c r="H5" s="95">
         <v>420</v>
       </c>
-      <c r="I5" s="98">
-        <v>0</v>
-      </c>
-      <c r="J5" s="98">
+      <c r="I5" s="95">
+        <v>0</v>
+      </c>
+      <c r="J5" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="98" t="s">
+      <c r="A6" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="98">
+      <c r="C6" s="95">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="D6" s="98">
+      <c r="D6" s="95">
         <v>0.13400000000000001</v>
       </c>
-      <c r="E6" s="98">
+      <c r="E6" s="95">
         <v>2.169</v>
       </c>
-      <c r="F6" s="98">
+      <c r="F6" s="95">
         <v>0.17199999999999999</v>
       </c>
-      <c r="G6" s="98">
+      <c r="G6" s="95">
         <v>0.13700000000000001</v>
       </c>
-      <c r="H6" s="98">
+      <c r="H6" s="95">
         <v>349</v>
       </c>
-      <c r="I6" s="98">
-        <v>0</v>
-      </c>
-      <c r="J6" s="98">
+      <c r="I6" s="95">
+        <v>0</v>
+      </c>
+      <c r="J6" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="98" t="s">
+      <c r="A7" s="95" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="98">
+      <c r="C7" s="95">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="D7" s="98">
+      <c r="D7" s="95">
         <v>0.112</v>
       </c>
-      <c r="E7" s="98">
+      <c r="E7" s="95">
         <v>1.496</v>
       </c>
-      <c r="F7" s="98">
+      <c r="F7" s="95">
         <v>0.16800000000000001</v>
       </c>
-      <c r="G7" s="98">
+      <c r="G7" s="95">
         <v>0.106</v>
       </c>
-      <c r="H7" s="98">
+      <c r="H7" s="95">
         <v>172</v>
       </c>
-      <c r="I7" s="98">
-        <v>0</v>
-      </c>
-      <c r="J7" s="98">
+      <c r="I7" s="95">
+        <v>0</v>
+      </c>
+      <c r="J7" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="98" t="s">
+      <c r="A8" s="95" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="98">
+      <c r="C8" s="95">
         <v>3.9E-2</v>
       </c>
-      <c r="D8" s="98">
+      <c r="D8" s="95">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="E8" s="98">
+      <c r="E8" s="95">
         <v>0.128</v>
       </c>
-      <c r="F8" s="98">
+      <c r="F8" s="95">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="G8" s="98">
+      <c r="G8" s="95">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="H8" s="98">
+      <c r="H8" s="95">
         <v>98</v>
       </c>
-      <c r="I8" s="98">
-        <v>0</v>
-      </c>
-      <c r="J8" s="98">
+      <c r="I8" s="95">
+        <v>0</v>
+      </c>
+      <c r="J8" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="98" t="s">
+      <c r="A9" s="95" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="98" t="s">
+      <c r="B9" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="98">
+      <c r="C9" s="95">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D9" s="98">
+      <c r="D9" s="95">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="E9" s="98">
+      <c r="E9" s="95">
         <v>0.13900000000000001</v>
       </c>
-      <c r="F9" s="98">
+      <c r="F9" s="95">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="G9" s="98">
+      <c r="G9" s="95">
         <v>0.104</v>
       </c>
-      <c r="H9" s="98">
+      <c r="H9" s="95">
         <v>280</v>
       </c>
-      <c r="I9" s="98">
-        <v>0</v>
-      </c>
-      <c r="J9" s="98">
+      <c r="I9" s="95">
+        <v>0</v>
+      </c>
+      <c r="J9" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="98" t="s">
+      <c r="A10" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="98" t="s">
+      <c r="B10" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="98">
+      <c r="C10" s="95">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="D10" s="98">
+      <c r="D10" s="95">
         <v>0.17</v>
       </c>
-      <c r="E10" s="98">
+      <c r="E10" s="95">
         <v>2.3929999999999998</v>
       </c>
-      <c r="F10" s="98">
+      <c r="F10" s="95">
         <v>0.25900000000000001</v>
       </c>
-      <c r="G10" s="98">
+      <c r="G10" s="95">
         <v>0.155</v>
       </c>
-      <c r="H10" s="98">
+      <c r="H10" s="95">
         <v>514</v>
       </c>
-      <c r="I10" s="98">
-        <v>0</v>
-      </c>
-      <c r="J10" s="98">
+      <c r="I10" s="95">
+        <v>0</v>
+      </c>
+      <c r="J10" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="98" t="s">
+      <c r="A11" s="95" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="98">
+      <c r="C11" s="95">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="D11" s="98">
+      <c r="D11" s="95">
         <v>0.14499999999999999</v>
       </c>
-      <c r="E11" s="98">
+      <c r="E11" s="95">
         <v>1.425</v>
       </c>
-      <c r="F11" s="98">
+      <c r="F11" s="95">
         <v>0.14299999999999999</v>
       </c>
-      <c r="G11" s="98">
+      <c r="G11" s="95">
         <v>0.158</v>
       </c>
-      <c r="H11" s="98">
+      <c r="H11" s="95">
         <v>98</v>
       </c>
-      <c r="I11" s="98">
-        <v>0</v>
-      </c>
-      <c r="J11" s="98">
+      <c r="I11" s="95">
+        <v>0</v>
+      </c>
+      <c r="J11" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="98" t="s">
+      <c r="A12" s="95" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="98">
+      <c r="C12" s="95">
         <v>0.109</v>
       </c>
-      <c r="D12" s="98">
+      <c r="D12" s="95">
         <v>0.19900000000000001</v>
       </c>
-      <c r="E12" s="98">
+      <c r="E12" s="95">
         <v>2.0259999999999998</v>
       </c>
-      <c r="F12" s="98">
+      <c r="F12" s="95">
         <v>0.20599999999999999</v>
       </c>
-      <c r="G12" s="98">
+      <c r="G12" s="95">
         <v>0.192</v>
       </c>
-      <c r="H12" s="98">
+      <c r="H12" s="95">
         <v>313</v>
       </c>
-      <c r="I12" s="98">
-        <v>0</v>
-      </c>
-      <c r="J12" s="98">
+      <c r="I12" s="95">
+        <v>0</v>
+      </c>
+      <c r="J12" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="98" t="s">
+      <c r="A13" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="98" t="s">
+      <c r="B13" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="98">
+      <c r="C13" s="95">
         <v>7.8E-2</v>
       </c>
-      <c r="D13" s="98">
+      <c r="D13" s="95">
         <v>0.157</v>
       </c>
-      <c r="E13" s="98">
+      <c r="E13" s="95">
         <v>1.873</v>
       </c>
-      <c r="F13" s="98">
+      <c r="F13" s="95">
         <v>0.248</v>
       </c>
-      <c r="G13" s="98">
+      <c r="G13" s="95">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H13" s="98">
+      <c r="H13" s="95">
         <v>97</v>
       </c>
-      <c r="I13" s="98">
-        <v>0</v>
-      </c>
-      <c r="J13" s="98">
+      <c r="I13" s="95">
+        <v>0</v>
+      </c>
+      <c r="J13" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="98" t="s">
+      <c r="A14" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="98">
+      <c r="C14" s="95">
         <v>0.6</v>
       </c>
-      <c r="D14" s="98">
+      <c r="D14" s="95">
         <v>0.96199999999999997</v>
       </c>
-      <c r="E14" s="98">
+      <c r="E14" s="95">
         <v>2.8860000000000001</v>
       </c>
-      <c r="F14" s="98">
+      <c r="F14" s="95">
         <v>0.45</v>
       </c>
-      <c r="G14" s="98">
+      <c r="G14" s="95">
         <v>1.746</v>
       </c>
-      <c r="H14" s="98">
+      <c r="H14" s="95">
         <v>173</v>
       </c>
-      <c r="I14" s="98">
-        <v>0</v>
-      </c>
-      <c r="J14" s="98">
+      <c r="I14" s="95">
+        <v>0</v>
+      </c>
+      <c r="J14" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="98" t="s">
+      <c r="A15" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="98" t="s">
+      <c r="B15" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="98">
+      <c r="C15" s="95">
         <v>0.38200000000000001</v>
       </c>
-      <c r="D15" s="98">
+      <c r="D15" s="95">
         <v>0.69099999999999995</v>
       </c>
-      <c r="E15" s="98">
+      <c r="E15" s="95">
         <v>2.762</v>
       </c>
-      <c r="F15" s="98">
+      <c r="F15" s="95">
         <v>0.44400000000000001</v>
       </c>
-      <c r="G15" s="98">
+      <c r="G15" s="95">
         <v>1.1299999999999999</v>
       </c>
-      <c r="H15" s="98">
+      <c r="H15" s="95">
         <v>98</v>
       </c>
-      <c r="I15" s="98">
-        <v>0</v>
-      </c>
-      <c r="J15" s="98">
+      <c r="I15" s="95">
+        <v>0</v>
+      </c>
+      <c r="J15" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="98" t="s">
+      <c r="A16" s="95" t="s">
         <v>79</v>
       </c>
-      <c r="B16" s="98" t="s">
+      <c r="B16" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="98">
+      <c r="C16" s="95">
         <v>0.47099999999999997</v>
       </c>
-      <c r="D16" s="98">
+      <c r="D16" s="95">
         <v>0.93700000000000006</v>
       </c>
-      <c r="E16" s="98">
+      <c r="E16" s="95">
         <v>3.6869999999999998</v>
       </c>
-      <c r="F16" s="98">
+      <c r="F16" s="95">
         <v>0.56799999999999995</v>
       </c>
-      <c r="G16" s="98">
+      <c r="G16" s="95">
         <v>1.885</v>
       </c>
-      <c r="H16" s="98">
+      <c r="H16" s="95">
         <v>108</v>
       </c>
-      <c r="I16" s="98">
-        <v>0</v>
-      </c>
-      <c r="J16" s="98">
+      <c r="I16" s="95">
+        <v>0</v>
+      </c>
+      <c r="J16" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="98" t="s">
+      <c r="A17" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="98" t="s">
+      <c r="B17" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="98">
+      <c r="C17" s="95">
         <v>0.42899999999999999</v>
       </c>
-      <c r="D17" s="98">
+      <c r="D17" s="95">
         <v>0.68400000000000005</v>
       </c>
-      <c r="E17" s="98">
+      <c r="E17" s="95">
         <v>2.9590000000000001</v>
       </c>
-      <c r="F17" s="98">
+      <c r="F17" s="95">
         <v>0.32900000000000001</v>
       </c>
-      <c r="G17" s="98">
+      <c r="G17" s="95">
         <v>0.83599999999999997</v>
       </c>
-      <c r="H17" s="98">
+      <c r="H17" s="95">
         <v>75</v>
       </c>
-      <c r="I17" s="98">
-        <v>0</v>
-      </c>
-      <c r="J17" s="98">
+      <c r="I17" s="95">
+        <v>0</v>
+      </c>
+      <c r="J17" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="98" t="s">
+      <c r="A18" s="95" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="98" t="s">
+      <c r="B18" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="98">
+      <c r="C18" s="95">
         <v>0.35</v>
       </c>
-      <c r="D18" s="98">
+      <c r="D18" s="95">
         <v>0.8</v>
       </c>
-      <c r="E18" s="98">
+      <c r="E18" s="95">
         <v>2.5880000000000001</v>
       </c>
-      <c r="F18" s="98">
+      <c r="F18" s="95">
         <v>0.621</v>
       </c>
-      <c r="G18" s="98">
+      <c r="G18" s="95">
         <v>1.714</v>
       </c>
-      <c r="H18" s="98">
+      <c r="H18" s="95">
         <v>32</v>
       </c>
-      <c r="I18" s="98">
-        <v>0</v>
-      </c>
-      <c r="J18" s="98">
+      <c r="I18" s="95">
+        <v>0</v>
+      </c>
+      <c r="J18" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="98" t="s">
+      <c r="A19" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="98" t="s">
+      <c r="B19" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="98">
+      <c r="C19" s="95">
         <v>0.38300000000000001</v>
       </c>
-      <c r="D19" s="98">
+      <c r="D19" s="95">
         <v>0.878</v>
       </c>
-      <c r="E19" s="98">
+      <c r="E19" s="95">
         <v>2.6549999999999998</v>
       </c>
-      <c r="F19" s="98">
+      <c r="F19" s="95">
         <v>0.69699999999999995</v>
       </c>
-      <c r="G19" s="98">
+      <c r="G19" s="95">
         <v>2.5070000000000001</v>
       </c>
-      <c r="H19" s="98">
+      <c r="H19" s="95">
         <v>36</v>
       </c>
-      <c r="I19" s="98">
-        <v>0</v>
-      </c>
-      <c r="J19" s="98">
+      <c r="I19" s="95">
+        <v>0</v>
+      </c>
+      <c r="J19" s="95">
         <v>0</v>
       </c>
     </row>
@@ -6714,8 +6828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6737,13 +6851,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E2" s="96" t="s">
+      <c r="E2" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E4" s="92" t="s">
@@ -7059,13 +7173,13 @@
       <c r="D17" s="72"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E22" s="96" t="s">
+      <c r="E22" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="96"/>
-      <c r="G22" s="96"/>
-      <c r="H22" s="96"/>
-      <c r="I22" s="96"/>
+      <c r="F22" s="98"/>
+      <c r="G22" s="98"/>
+      <c r="H22" s="98"/>
+      <c r="I22" s="98"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E24" s="92" t="s">

</xml_diff>